<commit_message>
Changes:  1) Added Dlib Face Recognition in Face_recognition.ipynb  2) Added Kunal Images in Training Data
</commit_message>
<xml_diff>
--- a/face_recognition/observation_logs.xlsx
+++ b/face_recognition/observation_logs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -812,6 +812,350 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>5</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2024-07-21-15-53-11</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2024-07-21</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>15:53:11</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>15:53:27</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>16.0748</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>53%</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>red</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>5</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2024-07-21-15-53-11</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2024-07-21</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>15:53:11</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>15:53:27</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>16.0748</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Michelle</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>86%</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>green</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>6</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2024-07-21-16-19-47</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2024-07-21</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>16:19:47</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>16:20:22</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>35.345559</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>52%</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>red</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>6</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2024-07-21-16-19-47</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2024-07-21</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>16:19:47</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>16:20:22</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>35.345559</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Kunal</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>79%</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>green</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>7</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2024-07-21-17-25-38</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2024-07-21</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>17:25:38</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>17:25:48</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>9.810617000000001</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>54%</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>red</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>7</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2024-07-21-17-25-38</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2024-07-21</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>17:25:38</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>17:25:48</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>9.810617000000001</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Kunal</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>88%</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>green</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>8</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2024-07-21-17-27-18</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2024-07-21</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>17:27:18</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>17:28:11</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>53.204704</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Kunal</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>84%</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>green</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>8</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2024-07-21-17-27-18</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2024-07-21</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>17:27:18</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>17:28:11</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>53.204704</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>52%</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>red</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>